<commit_message>
Implemented complete spencer and line of thrust
</commit_message>
<xml_diff>
--- a/thrust_calc_results.xlsx
+++ b/thrust_calc_results.xlsx
@@ -570,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>17126.73162235984</v>
+        <v>17126.73162235982</v>
       </c>
       <c r="C2" t="n">
         <v>14.10583813984129</v>
@@ -591,28 +591,28 @@
         <v>6976.910679550587</v>
       </c>
       <c r="I2" t="n">
-        <v>207.6712460492573</v>
+        <v>207.6712460492576</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2645344624757899</v>
+        <v>0.2645344624757903</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>20870.36326315546</v>
+        <v>20870.36326315545</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>3242.912335015562</v>
+        <v>3242.912335015547</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>20616.87615337186</v>
+        <v>20616.87615337185</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -624,19 +624,19 @@
         <v>39.99961494556892</v>
       </c>
       <c r="T2" t="n">
-        <v>35.79136578756066</v>
+        <v>35.79136578756065</v>
       </c>
       <c r="U2" t="n">
         <v>39.99961494556892</v>
       </c>
       <c r="V2" t="n">
-        <v>37.86130849572435</v>
+        <v>37.86130849572596</v>
       </c>
       <c r="W2" t="n">
         <v>39.99961494556892</v>
       </c>
       <c r="X2" t="n">
-        <v>36.8263371416425</v>
+        <v>36.82633714164331</v>
       </c>
       <c r="Y2" t="n">
         <v>0</v>
@@ -650,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>26393.52910615979</v>
+        <v>26393.52910615976</v>
       </c>
       <c r="C3" t="n">
         <v>12.77628929067389</v>
@@ -671,58 +671,58 @@
         <v>18718.16443016667</v>
       </c>
       <c r="I3" t="n">
-        <v>207.6712460492573</v>
+        <v>207.6712460492576</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2645344624757899</v>
+        <v>0.2645344624757903</v>
       </c>
       <c r="K3" t="n">
-        <v>20870.36326315546</v>
+        <v>20870.36326315545</v>
       </c>
       <c r="L3" t="n">
-        <v>52168.67746883237</v>
+        <v>52168.67746883234</v>
       </c>
       <c r="M3" t="n">
-        <v>3242.912335015562</v>
+        <v>3242.912335015547</v>
       </c>
       <c r="N3" t="n">
-        <v>8106.15730698816</v>
+        <v>8106.157306988123</v>
       </c>
       <c r="O3" t="n">
-        <v>20616.87615337186</v>
+        <v>20616.87615337185</v>
       </c>
       <c r="P3" t="n">
-        <v>51535.0475168251</v>
+        <v>51535.04751682508</v>
       </c>
       <c r="Q3" t="n">
-        <v>5.750682894377595</v>
+        <v>5.750682894377589</v>
       </c>
       <c r="R3" t="n">
-        <v>7.820625602541294</v>
+        <v>7.820625602542903</v>
       </c>
       <c r="S3" t="n">
-        <v>35.79136578756066</v>
+        <v>35.79136578756065</v>
       </c>
       <c r="T3" t="n">
         <v>31.05760450931817</v>
       </c>
       <c r="U3" t="n">
-        <v>37.86130849572435</v>
+        <v>37.86130849572596</v>
       </c>
       <c r="V3" t="n">
-        <v>31.89669480758798</v>
+        <v>31.89669480758862</v>
       </c>
       <c r="W3" t="n">
-        <v>36.8263371416425</v>
+        <v>36.82633714164331</v>
       </c>
       <c r="X3" t="n">
-        <v>31.47714965845308</v>
+        <v>31.4771496584534</v>
       </c>
       <c r="Y3" t="n">
         <v>2.91038304567337e-11</v>
       </c>
       <c r="Z3" t="n">
-        <v>2.91038304567337e-11</v>
+        <v>-2.91038304567337e-11</v>
       </c>
     </row>
     <row r="4">
@@ -730,7 +730,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>30590.57201577537</v>
+        <v>30590.57201577535</v>
       </c>
       <c r="C4" t="n">
         <v>11.87808673064982</v>
@@ -751,34 +751,34 @@
         <v>28137.86010431374</v>
       </c>
       <c r="I4" t="n">
-        <v>207.6712460492573</v>
+        <v>207.6712460492576</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2645344624757899</v>
+        <v>0.2645344624757903</v>
       </c>
       <c r="K4" t="n">
-        <v>52168.67746883237</v>
+        <v>52168.67746883234</v>
       </c>
       <c r="L4" t="n">
-        <v>86364.05951491569</v>
+        <v>86364.05951491563</v>
       </c>
       <c r="M4" t="n">
-        <v>8106.15730698816</v>
+        <v>8106.157306988123</v>
       </c>
       <c r="N4" t="n">
-        <v>13419.55913136287</v>
+        <v>13419.55913136281</v>
       </c>
       <c r="O4" t="n">
-        <v>51535.0475168251</v>
+        <v>51535.04751682508</v>
       </c>
       <c r="P4" t="n">
-        <v>85315.09953469993</v>
+        <v>85315.09953469987</v>
       </c>
       <c r="Q4" t="n">
-        <v>8.957275443468555</v>
+        <v>8.957275443468548</v>
       </c>
       <c r="R4" t="n">
-        <v>9.796365741738363</v>
+        <v>9.796365741739001</v>
       </c>
       <c r="S4" t="n">
         <v>31.05760450931817</v>
@@ -787,19 +787,19 @@
         <v>27.50954341761175</v>
       </c>
       <c r="U4" t="n">
-        <v>31.89669480758798</v>
+        <v>31.89669480758862</v>
       </c>
       <c r="V4" t="n">
-        <v>28.02075556401509</v>
+        <v>28.02075556401547</v>
       </c>
       <c r="W4" t="n">
-        <v>31.47714965845308</v>
+        <v>31.4771496584534</v>
       </c>
       <c r="X4" t="n">
-        <v>27.76514949081342</v>
+        <v>27.76514949081361</v>
       </c>
       <c r="Y4" t="n">
-        <v>0</v>
+        <v>-1.164153218269348e-10</v>
       </c>
       <c r="Z4" t="n">
         <v>-5.820766091346741e-11</v>
@@ -810,7 +810,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>32499.18525670046</v>
+        <v>32499.18525670044</v>
       </c>
       <c r="C5" t="n">
         <v>11.24349820547246</v>
@@ -831,58 +831,58 @@
         <v>35700.23289621456</v>
       </c>
       <c r="I5" t="n">
-        <v>207.6712460492573</v>
+        <v>207.6712460492576</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2645344624757899</v>
+        <v>0.2645344624757903</v>
       </c>
       <c r="K5" t="n">
-        <v>86364.05951491569</v>
+        <v>86364.05951491563</v>
       </c>
       <c r="L5" t="n">
-        <v>119813.6443566896</v>
+        <v>119813.6443566895</v>
       </c>
       <c r="M5" t="n">
-        <v>13419.55913136287</v>
+        <v>13419.55913136281</v>
       </c>
       <c r="N5" t="n">
-        <v>18617.0762956203</v>
+        <v>18617.07629562022</v>
       </c>
       <c r="O5" t="n">
-        <v>85315.09953469993</v>
+        <v>85315.09953469987</v>
       </c>
       <c r="P5" t="n">
-        <v>118358.4126466486</v>
+        <v>118358.4126466485</v>
       </c>
       <c r="Q5" t="n">
-        <v>11.79310929895033</v>
+        <v>11.79310929895032</v>
       </c>
       <c r="R5" t="n">
-        <v>12.30432144535367</v>
+        <v>12.30432144535405</v>
       </c>
       <c r="S5" t="n">
         <v>27.50954341761175</v>
       </c>
       <c r="T5" t="n">
-        <v>24.86079305563893</v>
+        <v>24.86079305563892</v>
       </c>
       <c r="U5" t="n">
-        <v>28.02075556401509</v>
+        <v>28.02075556401547</v>
       </c>
       <c r="V5" t="n">
-        <v>25.23125337377917</v>
+        <v>25.23125337377944</v>
       </c>
       <c r="W5" t="n">
-        <v>27.76514949081342</v>
+        <v>27.76514949081361</v>
       </c>
       <c r="X5" t="n">
-        <v>25.04602321470905</v>
+        <v>25.04602321470918</v>
       </c>
       <c r="Y5" t="n">
+        <v>5.820766091346741e-11</v>
+      </c>
+      <c r="Z5" t="n">
         <v>0</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>1.164153218269348e-10</v>
       </c>
     </row>
     <row r="6">
@@ -890,7 +890,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>33169.00469766768</v>
+        <v>33169.00469766767</v>
       </c>
       <c r="C6" t="n">
         <v>10.78695667671407</v>
@@ -911,55 +911,55 @@
         <v>41691.15558417432</v>
       </c>
       <c r="I6" t="n">
-        <v>207.6712460492573</v>
+        <v>207.6712460492576</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2645344624757899</v>
+        <v>0.2645344624757903</v>
       </c>
       <c r="K6" t="n">
-        <v>119813.6443566896</v>
+        <v>119813.6443566895</v>
       </c>
       <c r="L6" t="n">
-        <v>150512.412994593</v>
+        <v>150512.4129945929</v>
       </c>
       <c r="M6" t="n">
-        <v>18617.0762956203</v>
+        <v>18617.07629562022</v>
       </c>
       <c r="N6" t="n">
-        <v>23387.1617143728</v>
+        <v>23387.1617143727</v>
       </c>
       <c r="O6" t="n">
-        <v>118358.4126466486</v>
+        <v>118358.4126466485</v>
       </c>
       <c r="P6" t="n">
-        <v>148684.3203986241</v>
+        <v>148684.320398624</v>
       </c>
       <c r="Q6" t="n">
-        <v>14.24465094181203</v>
+        <v>14.24465094181202</v>
       </c>
       <c r="R6" t="n">
-        <v>14.61511125995228</v>
+        <v>14.61511125995254</v>
       </c>
       <c r="S6" t="n">
-        <v>24.86079305563893</v>
+        <v>24.86079305563892</v>
       </c>
       <c r="T6" t="n">
-        <v>22.9639266940214</v>
+        <v>22.96392669402138</v>
       </c>
       <c r="U6" t="n">
-        <v>25.23125337377917</v>
+        <v>25.23125337377944</v>
       </c>
       <c r="V6" t="n">
-        <v>23.25978009801216</v>
+        <v>23.25978009801236</v>
       </c>
       <c r="W6" t="n">
-        <v>25.04602321470905</v>
+        <v>25.04602321470918</v>
       </c>
       <c r="X6" t="n">
-        <v>23.11185339601678</v>
+        <v>23.11185339601687</v>
       </c>
       <c r="Y6" t="n">
-        <v>2.91038304567337e-10</v>
+        <v>3.492459654808044e-10</v>
       </c>
       <c r="Z6" t="n">
         <v>-1.164153218269348e-10</v>
@@ -991,58 +991,58 @@
         <v>46296.37332020365</v>
       </c>
       <c r="I7" t="n">
-        <v>207.6712460492573</v>
+        <v>207.6712460492576</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2645344624757899</v>
+        <v>0.2645344624757903</v>
       </c>
       <c r="K7" t="n">
-        <v>150512.412994593</v>
+        <v>150512.4129945929</v>
       </c>
       <c r="L7" t="n">
-        <v>177291.5195301109</v>
+        <v>177291.5195301108</v>
       </c>
       <c r="M7" t="n">
-        <v>23387.1617143728</v>
+        <v>23387.1617143727</v>
       </c>
       <c r="N7" t="n">
-        <v>27548.19589522189</v>
+        <v>27548.19589522177</v>
       </c>
       <c r="O7" t="n">
-        <v>148684.3203986241</v>
+        <v>148684.320398624</v>
       </c>
       <c r="P7" t="n">
-        <v>175138.1734523179</v>
+        <v>175138.1734523178</v>
       </c>
       <c r="Q7" t="n">
-        <v>16.33784048559878</v>
+        <v>16.33784048559876</v>
       </c>
       <c r="R7" t="n">
-        <v>16.63369388958954</v>
+        <v>16.63369388958974</v>
       </c>
       <c r="S7" t="n">
-        <v>22.9639266940214</v>
+        <v>22.96392669402138</v>
       </c>
       <c r="T7" t="n">
-        <v>21.72741049647512</v>
+        <v>21.7274104964751</v>
       </c>
       <c r="U7" t="n">
-        <v>23.25978009801216</v>
+        <v>23.25978009801236</v>
       </c>
       <c r="V7" t="n">
-        <v>21.97904466357365</v>
+        <v>21.97904466357381</v>
       </c>
       <c r="W7" t="n">
-        <v>23.11185339601678</v>
+        <v>23.11185339601687</v>
       </c>
       <c r="X7" t="n">
-        <v>21.85322758002438</v>
+        <v>21.85322758002446</v>
       </c>
       <c r="Y7" t="n">
-        <v>-2.91038304567337e-10</v>
+        <v>-2.328306436538696e-10</v>
       </c>
       <c r="Z7" t="n">
-        <v>5.820766091346741e-11</v>
+        <v>-1.164153218269348e-10</v>
       </c>
     </row>
     <row r="8">
@@ -1050,7 +1050,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>34936.28971150933</v>
+        <v>34936.28971150931</v>
       </c>
       <c r="C8" t="n">
         <v>10.07659006958534</v>
@@ -1071,58 +1071,58 @@
         <v>53576.08621085047</v>
       </c>
       <c r="I8" t="n">
-        <v>51.91781151231434</v>
+        <v>51.9178115123144</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3244184923225048</v>
+        <v>0.3244184923225052</v>
       </c>
       <c r="K8" t="n">
-        <v>177291.5195301109</v>
+        <v>177291.5195301108</v>
       </c>
       <c r="L8" t="n">
         <v>201589.3684865372</v>
       </c>
       <c r="M8" t="n">
-        <v>27548.19589522189</v>
+        <v>27548.19589522177</v>
       </c>
       <c r="N8" t="n">
-        <v>31323.68332213439</v>
+        <v>31323.68332213425</v>
       </c>
       <c r="O8" t="n">
-        <v>175138.1734523179</v>
+        <v>175138.1734523178</v>
       </c>
       <c r="P8" t="n">
         <v>199140.9057675884</v>
       </c>
       <c r="Q8" t="n">
-        <v>18.0954043779544</v>
+        <v>18.09540437795438</v>
       </c>
       <c r="R8" t="n">
-        <v>18.34703854505293</v>
+        <v>18.34703854505309</v>
       </c>
       <c r="S8" t="n">
-        <v>21.72741049647512</v>
+        <v>21.7274104964751</v>
       </c>
       <c r="T8" t="n">
-        <v>20.88124660072944</v>
+        <v>20.88124660072942</v>
       </c>
       <c r="U8" t="n">
-        <v>21.97904466357365</v>
+        <v>21.97904466357381</v>
       </c>
       <c r="V8" t="n">
-        <v>21.10277799855091</v>
+        <v>21.10277799855105</v>
       </c>
       <c r="W8" t="n">
-        <v>21.85322758002438</v>
+        <v>21.85322758002446</v>
       </c>
       <c r="X8" t="n">
-        <v>20.99201229964017</v>
+        <v>20.99201229964023</v>
       </c>
       <c r="Y8" t="n">
+        <v>5.820766091346741e-11</v>
+      </c>
+      <c r="Z8" t="n">
         <v>-5.820766091346741e-11</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>6.402842700481415e-10</v>
       </c>
     </row>
     <row r="9">
@@ -1130,7 +1130,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>38956.74174810763</v>
+        <v>38956.74174810761</v>
       </c>
       <c r="C9" t="n">
         <v>9.939495248171937</v>
@@ -1151,58 +1151,58 @@
         <v>65158.84795942099</v>
       </c>
       <c r="I9" t="n">
-        <v>51.91781151231434</v>
+        <v>51.9178115123144</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3244184923225048</v>
+        <v>0.3244184923225052</v>
       </c>
       <c r="K9" t="n">
         <v>201589.3684865372</v>
       </c>
       <c r="L9" t="n">
-        <v>223451.2939094524</v>
+        <v>223451.2939094523</v>
       </c>
       <c r="M9" t="n">
-        <v>31323.68332213439</v>
+        <v>31323.68332213425</v>
       </c>
       <c r="N9" t="n">
-        <v>34720.66816265808</v>
+        <v>34720.66816265794</v>
       </c>
       <c r="O9" t="n">
         <v>199140.9057675884</v>
       </c>
       <c r="P9" t="n">
-        <v>220737.3007720876</v>
+        <v>220737.3007720875</v>
       </c>
       <c r="Q9" t="n">
-        <v>19.29723182044357</v>
+        <v>19.29723182044355</v>
       </c>
       <c r="R9" t="n">
-        <v>19.51876321826504</v>
+        <v>19.51876321826518</v>
       </c>
       <c r="S9" t="n">
-        <v>20.88124660072944</v>
+        <v>20.88124660072942</v>
       </c>
       <c r="T9" t="n">
-        <v>20.41044569971111</v>
+        <v>20.41044569971109</v>
       </c>
       <c r="U9" t="n">
-        <v>21.10277799855091</v>
+        <v>21.10277799855105</v>
       </c>
       <c r="V9" t="n">
-        <v>20.61040540938281</v>
+        <v>20.61040540938293</v>
       </c>
       <c r="W9" t="n">
-        <v>20.99201229964017</v>
+        <v>20.99201229964023</v>
       </c>
       <c r="X9" t="n">
-        <v>20.51042555454696</v>
+        <v>20.51042555454701</v>
       </c>
       <c r="Y9" t="n">
-        <v>-4.074536263942719e-10</v>
+        <v>-2.91038304567337e-10</v>
       </c>
       <c r="Z9" t="n">
-        <v>4.074536263942719e-10</v>
+        <v>-1.164153218269348e-10</v>
       </c>
     </row>
     <row r="10">
@@ -1210,7 +1210,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>44324.77245843504</v>
+        <v>44324.77245843503</v>
       </c>
       <c r="C10" t="n">
         <v>9.874029601984471</v>
@@ -1231,58 +1231,58 @@
         <v>75659.45807402786</v>
       </c>
       <c r="I10" t="n">
-        <v>51.91781151231434</v>
+        <v>51.9178115123144</v>
       </c>
       <c r="J10" t="n">
-        <v>0.3244184923225048</v>
+        <v>0.3244184923225052</v>
       </c>
       <c r="K10" t="n">
-        <v>223451.2939094524</v>
+        <v>223451.2939094523</v>
       </c>
       <c r="L10" t="n">
         <v>241607.8345365945</v>
       </c>
       <c r="M10" t="n">
-        <v>34720.66816265808</v>
+        <v>34720.66816265794</v>
       </c>
       <c r="N10" t="n">
-        <v>37541.89694619906</v>
+        <v>37541.8969461989</v>
       </c>
       <c r="O10" t="n">
-        <v>220737.3007720876</v>
+        <v>220737.3007720875</v>
       </c>
       <c r="P10" t="n">
         <v>238673.3158171298</v>
       </c>
       <c r="Q10" t="n">
-        <v>20.02849989258322</v>
+        <v>20.02849989258319</v>
       </c>
       <c r="R10" t="n">
-        <v>20.22845960225492</v>
+        <v>20.22845960225504</v>
       </c>
       <c r="S10" t="n">
-        <v>20.41044569971111</v>
+        <v>20.41044569971109</v>
       </c>
       <c r="T10" t="n">
-        <v>20.38463223308759</v>
+        <v>20.38463223308755</v>
       </c>
       <c r="U10" t="n">
-        <v>20.61040540938281</v>
+        <v>20.61040540938293</v>
       </c>
       <c r="V10" t="n">
-        <v>20.56958952352878</v>
+        <v>20.56958952352887</v>
       </c>
       <c r="W10" t="n">
-        <v>20.51042555454696</v>
+        <v>20.51042555454701</v>
       </c>
       <c r="X10" t="n">
-        <v>20.47711087830818</v>
+        <v>20.47711087830821</v>
       </c>
       <c r="Y10" t="n">
-        <v>1.746229827404022e-10</v>
+        <v>2.328306436538696e-10</v>
       </c>
       <c r="Z10" t="n">
-        <v>5.820766091346741e-11</v>
+        <v>-4.074536263942719e-10</v>
       </c>
     </row>
     <row r="11">
@@ -1311,10 +1311,10 @@
         <v>108518.5126056569</v>
       </c>
       <c r="I11" t="n">
-        <v>103.8356230246287</v>
+        <v>103.8356230246288</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.2760519005232047</v>
       </c>
       <c r="K11" t="n">
         <v>241607.8345365945</v>
@@ -1323,10 +1323,10 @@
         <v>254320.3536140678</v>
       </c>
       <c r="M11" t="n">
-        <v>37541.89694619906</v>
+        <v>37541.8969461989</v>
       </c>
       <c r="N11" t="n">
-        <v>39517.21402169235</v>
+        <v>39517.2140216922</v>
       </c>
       <c r="O11" t="n">
         <v>238673.3158171298</v>
@@ -1335,34 +1335,34 @@
         <v>251231.4312707474</v>
       </c>
       <c r="Q11" t="n">
-        <v>20.38425723250165</v>
+        <v>20.38425723250162</v>
       </c>
       <c r="R11" t="n">
-        <v>20.56921452294284</v>
+        <v>20.56921452294294</v>
       </c>
       <c r="S11" t="n">
-        <v>20.38463223308759</v>
+        <v>20.38463223308755</v>
       </c>
       <c r="T11" t="n">
-        <v>21.2764542224214</v>
+        <v>21.27645422242136</v>
       </c>
       <c r="U11" t="n">
-        <v>20.56958952352878</v>
+        <v>20.56958952352887</v>
       </c>
       <c r="V11" t="n">
-        <v>21.45212167900722</v>
+        <v>21.45212167900729</v>
       </c>
       <c r="W11" t="n">
-        <v>20.47711087830818</v>
+        <v>20.47711087830821</v>
       </c>
       <c r="X11" t="n">
-        <v>21.36428795071431</v>
+        <v>21.36428795071433</v>
       </c>
       <c r="Y11" t="n">
-        <v>-6.984919309616089e-10</v>
+        <v>3.492459654808044e-10</v>
       </c>
       <c r="Z11" t="n">
-        <v>-4.656612873077393e-10</v>
+        <v>-5.820766091346741e-10</v>
       </c>
     </row>
     <row r="12">
@@ -1370,7 +1370,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>71242.4489983699</v>
+        <v>71242.44899836992</v>
       </c>
       <c r="C12" t="n">
         <v>12.50482896617596</v>
@@ -1391,10 +1391,10 @@
         <v>122436.3747918735</v>
       </c>
       <c r="I12" t="n">
-        <v>103.8356230246287</v>
+        <v>103.8356230246288</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.2760519005232047</v>
       </c>
       <c r="K12" t="n">
         <v>254320.3536140678</v>
@@ -1403,10 +1403,10 @@
         <v>256078.2094044913</v>
       </c>
       <c r="M12" t="n">
-        <v>39517.21402169235</v>
+        <v>39517.2140216922</v>
       </c>
       <c r="N12" t="n">
-        <v>39790.3559959869</v>
+        <v>39790.35599598675</v>
       </c>
       <c r="O12" t="n">
         <v>251231.4312707474</v>
@@ -1415,34 +1415,34 @@
         <v>252967.9365088056</v>
       </c>
       <c r="Q12" t="n">
-        <v>20.60783106858035</v>
+        <v>20.60783106858031</v>
       </c>
       <c r="R12" t="n">
-        <v>20.78349852516616</v>
+        <v>20.78349852516624</v>
       </c>
       <c r="S12" t="n">
-        <v>21.2764542224214</v>
+        <v>21.27645422242136</v>
       </c>
       <c r="T12" t="n">
-        <v>23.07765734025184</v>
+        <v>23.07765734025179</v>
       </c>
       <c r="U12" t="n">
-        <v>21.45212167900722</v>
+        <v>21.45212167900729</v>
       </c>
       <c r="V12" t="n">
-        <v>23.25210014250314</v>
+        <v>23.2521001425032</v>
       </c>
       <c r="W12" t="n">
-        <v>21.36428795071431</v>
+        <v>21.36428795071433</v>
       </c>
       <c r="X12" t="n">
-        <v>23.16487874137749</v>
+        <v>23.1648787413775</v>
       </c>
       <c r="Y12" t="n">
-        <v>0</v>
+        <v>-2.328306436538696e-10</v>
       </c>
       <c r="Z12" t="n">
-        <v>3.492459654808044e-10</v>
+        <v>6.984919309616089e-10</v>
       </c>
     </row>
     <row r="13">
@@ -1471,22 +1471,22 @@
         <v>101962.1203276141</v>
       </c>
       <c r="I13" t="n">
-        <v>103.8356230246287</v>
+        <v>103.8356230246288</v>
       </c>
       <c r="J13" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.2760519005232047</v>
       </c>
       <c r="K13" t="n">
         <v>256078.2094044913</v>
       </c>
       <c r="L13" t="n">
-        <v>247679.9309536193</v>
+        <v>247679.9309536194</v>
       </c>
       <c r="M13" t="n">
-        <v>39790.3559959869</v>
+        <v>39790.35599598675</v>
       </c>
       <c r="N13" t="n">
-        <v>38485.40119295727</v>
+        <v>38485.40119295712</v>
       </c>
       <c r="O13" t="n">
         <v>252967.9365088056</v>
@@ -1495,25 +1495,25 @@
         <v>244671.6618086508</v>
       </c>
       <c r="Q13" t="n">
-        <v>20.44460328330686</v>
+        <v>20.44460328330682</v>
       </c>
       <c r="R13" t="n">
-        <v>20.61904608555816</v>
+        <v>20.61904608555823</v>
       </c>
       <c r="S13" t="n">
-        <v>23.07765734025184</v>
+        <v>23.07765734025179</v>
       </c>
       <c r="T13" t="n">
-        <v>25.31730615616783</v>
+        <v>25.31730615616778</v>
       </c>
       <c r="U13" t="n">
-        <v>23.25210014250314</v>
+        <v>23.2521001425032</v>
       </c>
       <c r="V13" t="n">
-        <v>25.49774886306175</v>
+        <v>25.49774886306181</v>
       </c>
       <c r="W13" t="n">
-        <v>23.16487874137749</v>
+        <v>23.1648787413775</v>
       </c>
       <c r="X13" t="n">
         <v>25.40752750961479</v>
@@ -1522,7 +1522,7 @@
         <v>-4.074536263942719e-10</v>
       </c>
       <c r="Z13" t="n">
-        <v>5.820766091346741e-11</v>
+        <v>5.820766091346741e-10</v>
       </c>
     </row>
     <row r="14">
@@ -1551,58 +1551,58 @@
         <v>97988.89922008957</v>
       </c>
       <c r="I14" t="n">
-        <v>103.8356230246287</v>
+        <v>103.8356230246288</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.2760519005232047</v>
       </c>
       <c r="K14" t="n">
-        <v>247679.9309536193</v>
+        <v>247679.9309536194</v>
       </c>
       <c r="L14" t="n">
-        <v>230608.4400432078</v>
+        <v>230608.4400432079</v>
       </c>
       <c r="M14" t="n">
-        <v>38485.40119295727</v>
+        <v>38485.40119295712</v>
       </c>
       <c r="N14" t="n">
-        <v>35832.77134878899</v>
+        <v>35832.77134878885</v>
       </c>
       <c r="O14" t="n">
         <v>244671.6618086508</v>
       </c>
       <c r="P14" t="n">
-        <v>227807.5176912017</v>
+        <v>227807.5176912018</v>
       </c>
       <c r="Q14" t="n">
-        <v>20.11807051736288</v>
+        <v>20.11807051736283</v>
       </c>
       <c r="R14" t="n">
-        <v>20.2985132242568</v>
+        <v>20.29851322425686</v>
       </c>
       <c r="S14" t="n">
-        <v>25.31730615616783</v>
+        <v>25.31730615616778</v>
       </c>
       <c r="T14" t="n">
-        <v>28.29791067679702</v>
+        <v>28.29791067679695</v>
       </c>
       <c r="U14" t="n">
-        <v>25.49774886306175</v>
+        <v>25.49774886306181</v>
       </c>
       <c r="V14" t="n">
-        <v>28.49199306897803</v>
+        <v>28.49199306897808</v>
       </c>
       <c r="W14" t="n">
         <v>25.40752750961479</v>
       </c>
       <c r="X14" t="n">
-        <v>28.39495187288752</v>
+        <v>28.39495187288751</v>
       </c>
       <c r="Y14" t="n">
         <v>0</v>
       </c>
       <c r="Z14" t="n">
-        <v>3.492459654808044e-10</v>
+        <v>-2.328306436538696e-10</v>
       </c>
     </row>
     <row r="15">
@@ -1631,58 +1631,58 @@
         <v>92723.7348333438</v>
       </c>
       <c r="I15" t="n">
-        <v>103.8356230246287</v>
+        <v>103.8356230246288</v>
       </c>
       <c r="J15" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.2760519005232047</v>
       </c>
       <c r="K15" t="n">
-        <v>230608.4400432078</v>
+        <v>230608.4400432079</v>
       </c>
       <c r="L15" t="n">
-        <v>205705.6884024436</v>
+        <v>205705.6884024437</v>
       </c>
       <c r="M15" t="n">
-        <v>35832.77134878899</v>
+        <v>35832.77134878885</v>
       </c>
       <c r="N15" t="n">
-        <v>31963.29196055848</v>
+        <v>31963.29196055836</v>
       </c>
       <c r="O15" t="n">
-        <v>227807.5176912017</v>
+        <v>227807.5176912018</v>
       </c>
       <c r="P15" t="n">
-        <v>203207.2297143173</v>
+        <v>203207.2297143174</v>
       </c>
       <c r="Q15" t="n">
-        <v>19.58957551278434</v>
+        <v>19.58957551278426</v>
       </c>
       <c r="R15" t="n">
-        <v>19.78365790496535</v>
+        <v>19.78365790496539</v>
       </c>
       <c r="S15" t="n">
-        <v>28.29791067679702</v>
+        <v>28.29791067679695</v>
       </c>
       <c r="T15" t="n">
-        <v>32.05207099696817</v>
+        <v>32.05207099696808</v>
       </c>
       <c r="U15" t="n">
-        <v>28.49199306897803</v>
+        <v>28.49199306897808</v>
       </c>
       <c r="V15" t="n">
-        <v>32.2703389781734</v>
+        <v>32.27033897817344</v>
       </c>
       <c r="W15" t="n">
-        <v>28.39495187288752</v>
+        <v>28.39495187288751</v>
       </c>
       <c r="X15" t="n">
-        <v>32.16120498757078</v>
+        <v>32.16120498757076</v>
       </c>
       <c r="Y15" t="n">
-        <v>1.164153218269348e-10</v>
+        <v>5.820766091346741e-10</v>
       </c>
       <c r="Z15" t="n">
-        <v>1.746229827404022e-10</v>
+        <v>-5.820766091346741e-10</v>
       </c>
     </row>
     <row r="16">
@@ -1690,7 +1690,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>43474.14387046653</v>
+        <v>43474.14387046656</v>
       </c>
       <c r="C16" t="n">
         <v>11.46400365670253</v>
@@ -1711,58 +1711,58 @@
         <v>86017.22004816629</v>
       </c>
       <c r="I16" t="n">
-        <v>103.8356230246287</v>
+        <v>103.8356230246288</v>
       </c>
       <c r="J16" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.2760519005232047</v>
       </c>
       <c r="K16" t="n">
-        <v>205705.6884024436</v>
+        <v>205705.6884024437</v>
       </c>
       <c r="L16" t="n">
-        <v>173940.9557781213</v>
+        <v>173940.9557781214</v>
       </c>
       <c r="M16" t="n">
-        <v>31963.29196055848</v>
+        <v>31963.29196055836</v>
       </c>
       <c r="N16" t="n">
-        <v>27027.57321206212</v>
+        <v>27027.57321206203</v>
       </c>
       <c r="O16" t="n">
-        <v>203207.2297143173</v>
+        <v>203207.2297143174</v>
       </c>
       <c r="P16" t="n">
-        <v>171828.3049537327</v>
+        <v>171828.3049537329</v>
       </c>
       <c r="Q16" t="n">
-        <v>18.79876880141228</v>
+        <v>18.79876880141219</v>
       </c>
       <c r="R16" t="n">
-        <v>19.01703678261751</v>
+        <v>19.01703678261755</v>
       </c>
       <c r="S16" t="n">
-        <v>32.05207099696817</v>
+        <v>32.05207099696808</v>
       </c>
       <c r="T16" t="n">
-        <v>36.66815005009166</v>
+        <v>36.66815005009155</v>
       </c>
       <c r="U16" t="n">
-        <v>32.2703389781734</v>
+        <v>32.27033897817344</v>
       </c>
       <c r="V16" t="n">
-        <v>36.92786541911432</v>
+        <v>36.92786541911435</v>
       </c>
       <c r="W16" t="n">
-        <v>32.16120498757078</v>
+        <v>32.16120498757076</v>
       </c>
       <c r="X16" t="n">
-        <v>36.79800773460299</v>
+        <v>36.79800773460295</v>
       </c>
       <c r="Y16" t="n">
-        <v>-1.164153218269348e-10</v>
+        <v>2.328306436538696e-10</v>
       </c>
       <c r="Z16" t="n">
-        <v>2.91038304567337e-10</v>
+        <v>-5.820766091346741e-10</v>
       </c>
     </row>
     <row r="17">
@@ -1770,7 +1770,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>38503.67616132362</v>
+        <v>38503.67616132366</v>
       </c>
       <c r="C17" t="n">
         <v>12.21319636798589</v>
@@ -1791,58 +1791,58 @@
         <v>77643.23955338272</v>
       </c>
       <c r="I17" t="n">
-        <v>103.8356230246287</v>
+        <v>103.8356230246288</v>
       </c>
       <c r="J17" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.2760519005232047</v>
       </c>
       <c r="K17" t="n">
-        <v>173940.9557781213</v>
+        <v>173940.9557781214</v>
       </c>
       <c r="L17" t="n">
-        <v>136793.6190736684</v>
+        <v>136793.6190736686</v>
       </c>
       <c r="M17" t="n">
-        <v>27027.57321206212</v>
+        <v>27027.57321206203</v>
       </c>
       <c r="N17" t="n">
-        <v>21255.48602350242</v>
+        <v>21255.48602350236</v>
       </c>
       <c r="O17" t="n">
-        <v>171828.3049537327</v>
+        <v>171828.3049537329</v>
       </c>
       <c r="P17" t="n">
-        <v>135132.1521073967</v>
+        <v>135132.1521073968</v>
       </c>
       <c r="Q17" t="n">
-        <v>17.69430502234309</v>
+        <v>17.69430502234298</v>
       </c>
       <c r="R17" t="n">
-        <v>17.95402039136575</v>
+        <v>17.95402039136578</v>
       </c>
       <c r="S17" t="n">
-        <v>36.66815005009166</v>
+        <v>36.66815005009155</v>
       </c>
       <c r="T17" t="n">
-        <v>42.2815437463728</v>
+        <v>42.28154374637266</v>
       </c>
       <c r="U17" t="n">
-        <v>36.92786541911432</v>
+        <v>36.92786541911435</v>
       </c>
       <c r="V17" t="n">
-        <v>42.61557024220299</v>
+        <v>42.61557024220302</v>
       </c>
       <c r="W17" t="n">
-        <v>36.79800773460299</v>
+        <v>36.79800773460295</v>
       </c>
       <c r="X17" t="n">
-        <v>42.4485569942879</v>
+        <v>42.44855699428784</v>
       </c>
       <c r="Y17" t="n">
-        <v>-1.164153218269348e-10</v>
+        <v>1.746229827404022e-10</v>
       </c>
       <c r="Z17" t="n">
-        <v>-4.074536263942719e-10</v>
+        <v>-4.656612873077393e-10</v>
       </c>
     </row>
     <row r="18">
@@ -1850,7 +1850,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>33106.3700149315</v>
+        <v>33106.37001493154</v>
       </c>
       <c r="C18" t="n">
         <v>13.291644383338</v>
@@ -1871,58 +1871,58 @@
         <v>67246.54663088753</v>
       </c>
       <c r="I18" t="n">
-        <v>103.8356230246287</v>
+        <v>103.8356230246288</v>
       </c>
       <c r="J18" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.2760519005232047</v>
       </c>
       <c r="K18" t="n">
-        <v>136793.6190736684</v>
+        <v>136793.6190736686</v>
       </c>
       <c r="L18" t="n">
-        <v>96258.81121913625</v>
+        <v>96258.81121913638</v>
       </c>
       <c r="M18" t="n">
-        <v>21255.48602350242</v>
+        <v>21255.48602350236</v>
       </c>
       <c r="N18" t="n">
-        <v>14957.04134712195</v>
+        <v>14957.04134712191</v>
       </c>
       <c r="O18" t="n">
-        <v>135132.1521073967</v>
+        <v>135132.1521073968</v>
       </c>
       <c r="P18" t="n">
-        <v>95089.67163399921</v>
+        <v>95089.67163399936</v>
       </c>
       <c r="Q18" t="n">
-        <v>16.19700653572335</v>
+        <v>16.19700653572321</v>
       </c>
       <c r="R18" t="n">
-        <v>16.53103303155354</v>
+        <v>16.53103303155358</v>
       </c>
       <c r="S18" t="n">
-        <v>42.2815437463728</v>
+        <v>42.28154374637266</v>
       </c>
       <c r="T18" t="n">
-        <v>49.12654870122714</v>
+        <v>49.12654870122692</v>
       </c>
       <c r="U18" t="n">
-        <v>42.61557024220299</v>
+        <v>42.61557024220302</v>
       </c>
       <c r="V18" t="n">
-        <v>49.61149188961511</v>
+        <v>49.61149188961513</v>
       </c>
       <c r="W18" t="n">
-        <v>42.4485569942879</v>
+        <v>42.44855699428784</v>
       </c>
       <c r="X18" t="n">
-        <v>49.36902029542112</v>
+        <v>49.36902029542102</v>
       </c>
       <c r="Y18" t="n">
-        <v>5.820766091346741e-11</v>
+        <v>0</v>
       </c>
       <c r="Z18" t="n">
-        <v>-5.820766091346741e-11</v>
+        <v>1.164153218269348e-10</v>
       </c>
     </row>
     <row r="19">
@@ -1930,7 +1930,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>26610.08740263997</v>
+        <v>26610.08740263999</v>
       </c>
       <c r="C19" t="n">
         <v>14.94422825432905</v>
@@ -1951,58 +1951,58 @@
         <v>54248.53262366771</v>
       </c>
       <c r="I19" t="n">
-        <v>103.8356230246287</v>
+        <v>103.8356230246288</v>
       </c>
       <c r="J19" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.2760519005232047</v>
       </c>
       <c r="K19" t="n">
-        <v>96258.81121913625</v>
+        <v>96258.81121913638</v>
       </c>
       <c r="L19" t="n">
-        <v>55367.76596963337</v>
+        <v>55367.7659696335</v>
       </c>
       <c r="M19" t="n">
-        <v>14957.04134712195</v>
+        <v>14957.04134712191</v>
       </c>
       <c r="N19" t="n">
-        <v>8603.243219161472</v>
+        <v>8603.243219161457</v>
       </c>
       <c r="O19" t="n">
-        <v>95089.67163399921</v>
+        <v>95089.67163399936</v>
       </c>
       <c r="P19" t="n">
-        <v>54695.28055125089</v>
+        <v>54695.28055125102</v>
       </c>
       <c r="Q19" t="n">
-        <v>14.19327533117855</v>
+        <v>14.19327533117833</v>
       </c>
       <c r="R19" t="n">
-        <v>14.67821851956651</v>
+        <v>14.67821851956653</v>
       </c>
       <c r="S19" t="n">
-        <v>49.12654870122714</v>
+        <v>49.12654870122692</v>
       </c>
       <c r="T19" t="n">
-        <v>57.59224287273218</v>
+        <v>57.59224287273177</v>
       </c>
       <c r="U19" t="n">
-        <v>49.61149188961511</v>
+        <v>49.61149188961513</v>
       </c>
       <c r="V19" t="n">
-        <v>58.47187038671452</v>
+        <v>58.47187038671453</v>
       </c>
       <c r="W19" t="n">
-        <v>49.36902029542112</v>
+        <v>49.36902029542102</v>
       </c>
       <c r="X19" t="n">
-        <v>58.03205662972335</v>
+        <v>58.03205662972315</v>
       </c>
       <c r="Y19" t="n">
+        <v>5.820766091346741e-11</v>
+      </c>
+      <c r="Z19" t="n">
         <v>-5.820766091346741e-11</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -2010,7 +2010,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>19840.17967533819</v>
+        <v>19840.1796753382</v>
       </c>
       <c r="C20" t="n">
         <v>17.80010592668061</v>
@@ -2031,58 +2031,58 @@
         <v>38974.45926823906</v>
       </c>
       <c r="I20" t="n">
-        <v>103.8356230246287</v>
+        <v>103.8356230246288</v>
       </c>
       <c r="J20" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.2760519005232047</v>
       </c>
       <c r="K20" t="n">
-        <v>55367.76596963337</v>
+        <v>55367.7659696335</v>
       </c>
       <c r="L20" t="n">
-        <v>18621.69573402152</v>
+        <v>18621.69573402165</v>
       </c>
       <c r="M20" t="n">
-        <v>8603.243219161472</v>
+        <v>8603.243219161457</v>
       </c>
       <c r="N20" t="n">
-        <v>2893.506262125055</v>
+        <v>2893.506262125064</v>
       </c>
       <c r="O20" t="n">
-        <v>54695.28055125089</v>
+        <v>54695.28055125102</v>
       </c>
       <c r="P20" t="n">
-        <v>18395.52047433065</v>
+        <v>18395.52047433078</v>
       </c>
       <c r="Q20" t="n">
-        <v>11.45011634786243</v>
+        <v>11.45011634786202</v>
       </c>
       <c r="R20" t="n">
-        <v>12.32974386184477</v>
+        <v>12.32974386184478</v>
       </c>
       <c r="S20" t="n">
-        <v>57.59224287273218</v>
+        <v>57.59224287273177</v>
       </c>
       <c r="T20" t="n">
-        <v>68.45977037954877</v>
+        <v>68.45977037954749</v>
       </c>
       <c r="U20" t="n">
-        <v>58.47187038671452</v>
+        <v>58.47187038671453</v>
       </c>
       <c r="V20" t="n">
-        <v>71.33892802852256</v>
+        <v>71.3389280285225</v>
       </c>
       <c r="W20" t="n">
-        <v>58.03205662972335</v>
+        <v>58.03205662972315</v>
       </c>
       <c r="X20" t="n">
-        <v>69.89934920403567</v>
+        <v>69.89934920403499</v>
       </c>
       <c r="Y20" t="n">
         <v>0</v>
       </c>
       <c r="Z20" t="n">
-        <v>0</v>
+        <v>1.164153218269348e-10</v>
       </c>
     </row>
     <row r="21">
@@ -2090,7 +2090,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>10045.72056946627</v>
+        <v>10045.72056946628</v>
       </c>
       <c r="C21" t="n">
         <v>24.28436213742816</v>
@@ -2111,49 +2111,49 @@
         <v>16948.91230046818</v>
       </c>
       <c r="I21" t="n">
-        <v>103.8356230246287</v>
+        <v>103.8356230246288</v>
       </c>
       <c r="J21" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.2760519005232047</v>
       </c>
       <c r="K21" t="n">
-        <v>18621.69573402152</v>
+        <v>18621.69573402165</v>
       </c>
       <c r="L21" t="n">
         <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>2893.506262125055</v>
+        <v>2893.506262125064</v>
       </c>
       <c r="N21" t="n">
         <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>18395.52047433065</v>
+        <v>18395.52047433078</v>
       </c>
       <c r="P21" t="n">
         <v>0</v>
       </c>
       <c r="Q21" t="n">
-        <v>7.417608154846183</v>
+        <v>7.417608154844906</v>
       </c>
       <c r="R21" t="n">
-        <v>10.29676580381998</v>
+        <v>10.29676580381991</v>
       </c>
       <c r="S21" t="n">
-        <v>68.45977037954877</v>
+        <v>68.45977037954749</v>
       </c>
       <c r="T21" t="n">
         <v>83.95181749179723</v>
       </c>
       <c r="U21" t="n">
-        <v>71.33892802852256</v>
+        <v>71.3389280285225</v>
       </c>
       <c r="V21" t="n">
         <v>83.95181749179723</v>
       </c>
       <c r="W21" t="n">
-        <v>69.89934920403567</v>
+        <v>69.89934920403499</v>
       </c>
       <c r="X21" t="n">
         <v>83.95181749179723</v>

</xml_diff>